<commit_message>
I like Suicide very much
</commit_message>
<xml_diff>
--- a/Task & work time documentation.xlsx
+++ b/Task & work time documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FH\GitRepo\FH_BIF5_CGRMR_OpenGL-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F6E20C-5C51-41C2-8AE7-2BB1233E1200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76080EA4-89A5-4755-8DB2-CF8AD2ECD8E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36000" yWindow="345" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -370,13 +370,13 @@
   <dimension ref="B1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
changed readme.md, tried to fix ref issue
ref issue was NOT resolved added time
</commit_message>
<xml_diff>
--- a/Task & work time documentation.xlsx
+++ b/Task & work time documentation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studium\FH\Sem_5\FH_BIF5_CGRMR_OpenGL-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FH_BIF5_CGRMR_OpenGL-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9DFDDA4-3FFD-4DBD-A06B-7D97FEE06E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D428D64-36B1-4E29-A897-E7928A0DFEC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>Flo</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Moving Cube on Grid</t>
+  </si>
+  <si>
+    <t>fixing ref / dependency issues of poppinger</t>
   </si>
 </sst>
 </file>
@@ -93,7 +96,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -374,15 +377,18 @@
   <dimension ref="B1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" customWidth="1"/>
+    <col min="11" max="11" width="15" customWidth="1"/>
+    <col min="12" max="12" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.25">
@@ -444,6 +450,15 @@
       <c r="H3" s="2">
         <v>45678</v>
       </c>
+      <c r="J3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="1">
+        <v>45678</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>